<commit_message>
Consolidated Room AC options. Several bugfixes.
</commit_message>
<xml_diff>
--- a/projects/resstock_testing.xlsx
+++ b/projects/resstock_testing.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="437">
   <si>
     <t>type</t>
   </si>
@@ -855,15 +855,6 @@
     <t>Location EPW</t>
   </si>
   <si>
-    <t>Vintage</t>
-  </si>
-  <si>
-    <t>Heating Fuel</t>
-  </si>
-  <si>
-    <t>Usage Level</t>
-  </si>
-  <si>
     <t>Geometry Foundation Type</t>
   </si>
   <si>
@@ -1101,15 +1092,6 @@
     <t>building_characteristics_report.Location EPW</t>
   </si>
   <si>
-    <t>building_characteristics_report.Vintage</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Heating Fuel</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Usage Level</t>
-  </si>
-  <si>
     <t>building_characteristics_report.Geometry Foundation Type</t>
   </si>
   <si>
@@ -1357,18 +1339,6 @@
   </si>
   <si>
     <t>[1]</t>
-  </si>
-  <si>
-    <t>Location Heating Region</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Location Heating Region</t>
-  </si>
-  <si>
-    <t>Location Cooling Region</t>
-  </si>
-  <si>
-    <t>building_characteristics_report.Location Cooling Region</t>
   </si>
   <si>
     <t>ResStock_Testing</t>
@@ -5512,7 +5482,7 @@
         <v>73</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>153</v>
@@ -5623,7 +5593,7 @@
         <v>34</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>445</v>
+        <v>435</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>75</v>
@@ -5645,7 +5615,7 @@
         <v>21</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="F15" s="21" t="s">
         <v>154</v>
@@ -5739,19 +5709,19 @@
         <v>1000</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="E24" s="21"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="21" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="B25" s="20">
         <v>1</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="D25" s="25"/>
       <c r="E25" s="21"/>
@@ -5815,7 +5785,7 @@
         <v>24</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>446</v>
+        <v>436</v>
       </c>
     </row>
     <row r="37" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -6212,7 +6182,7 @@
       <c r="P5" s="44"/>
       <c r="Q5" s="44"/>
       <c r="R5" s="44" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="S5" s="44"/>
       <c r="T5" s="44"/>
@@ -6226,16 +6196,16 @@
         <v>1</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="C6" s="51" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="D6" s="51" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="E6" s="51" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="F6" s="51"/>
       <c r="G6" s="51"/>
@@ -6266,7 +6236,7 @@
       </c>
       <c r="C7" s="52"/>
       <c r="D7" s="52" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="E7" s="52" t="str">
         <f>LOWER(SUBSTITUTE(D7," ","_"))</f>
@@ -6295,7 +6265,7 @@
       </c>
       <c r="O7" s="52"/>
       <c r="P7" s="52" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="Q7" s="52"/>
       <c r="R7" s="52" t="s">
@@ -6315,13 +6285,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E8" s="39" t="s">
         <v>234</v>
@@ -6351,13 +6321,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="E9" s="39" t="s">
         <v>234</v>
@@ -6436,11 +6406,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M127"/>
+  <dimension ref="A1:M122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6556,12 +6526,12 @@
     </row>
     <row r="4" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="47" t="s">
-        <v>441</v>
+        <v>272</v>
       </c>
       <c r="B4" s="47"/>
       <c r="C4" s="47"/>
       <c r="D4" s="47" t="s">
-        <v>442</v>
+        <v>351</v>
       </c>
       <c r="E4" s="47"/>
       <c r="F4" s="47" t="s">
@@ -6583,12 +6553,12 @@
     </row>
     <row r="5" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="47" t="s">
-        <v>443</v>
+        <v>273</v>
       </c>
       <c r="B5" s="47"/>
       <c r="C5" s="47"/>
       <c r="D5" s="47" t="s">
-        <v>444</v>
+        <v>352</v>
       </c>
       <c r="E5" s="47"/>
       <c r="F5" s="47" t="s">
@@ -6610,12 +6580,12 @@
     </row>
     <row r="6" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B6" s="47"/>
       <c r="C6" s="47"/>
       <c r="D6" s="47" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E6" s="47"/>
       <c r="F6" s="47" t="s">
@@ -6637,12 +6607,12 @@
     </row>
     <row r="7" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="47" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B7" s="47"/>
       <c r="C7" s="47"/>
       <c r="D7" s="47" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E7" s="47"/>
       <c r="F7" s="47" t="s">
@@ -6664,12 +6634,12 @@
     </row>
     <row r="8" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="47" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B8" s="47"/>
       <c r="C8" s="47"/>
       <c r="D8" s="47" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E8" s="47"/>
       <c r="F8" s="47" t="s">
@@ -6691,12 +6661,12 @@
     </row>
     <row r="9" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="47" t="s">
-        <v>275</v>
+        <v>423</v>
       </c>
       <c r="B9" s="47"/>
       <c r="C9" s="47"/>
       <c r="D9" s="47" t="s">
-        <v>357</v>
+        <v>424</v>
       </c>
       <c r="E9" s="47"/>
       <c r="F9" s="47" t="s">
@@ -6718,12 +6688,12 @@
     </row>
     <row r="10" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="47" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B10" s="47"/>
       <c r="C10" s="47"/>
       <c r="D10" s="47" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="E10" s="47"/>
       <c r="F10" s="47" t="s">
@@ -6745,12 +6715,12 @@
     </row>
     <row r="11" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="47" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B11" s="47"/>
       <c r="C11" s="47"/>
       <c r="D11" s="47" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="E11" s="47"/>
       <c r="F11" s="47" t="s">
@@ -6772,12 +6742,12 @@
     </row>
     <row r="12" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B12" s="47"/>
       <c r="C12" s="47"/>
       <c r="D12" s="47" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="E12" s="47"/>
       <c r="F12" s="47" t="s">
@@ -6799,14 +6769,11 @@
     </row>
     <row r="13" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47" t="s">
-        <v>279</v>
-      </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="47"/>
+        <v>280</v>
+      </c>
       <c r="D13" s="47" t="s">
-        <v>361</v>
-      </c>
-      <c r="E13" s="47"/>
+        <v>359</v>
+      </c>
       <c r="F13" s="47" t="s">
         <v>240</v>
       </c>
@@ -6819,21 +6786,14 @@
       <c r="I13" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="J13" s="47"/>
-      <c r="K13" s="47"/>
-      <c r="L13" s="47"/>
-      <c r="M13" s="47"/>
     </row>
     <row r="14" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="47" t="s">
-        <v>429</v>
-      </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
+        <v>281</v>
+      </c>
       <c r="D14" s="47" t="s">
-        <v>430</v>
-      </c>
-      <c r="E14" s="47"/>
+        <v>360</v>
+      </c>
       <c r="F14" s="47" t="s">
         <v>240</v>
       </c>
@@ -6846,19 +6806,15 @@
       <c r="I14" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="J14" s="47"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="47"/>
     </row>
     <row r="15" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="47" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="B15" s="47"/>
       <c r="C15" s="47"/>
       <c r="D15" s="47" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E15" s="47"/>
       <c r="F15" s="47" t="s">
@@ -6880,12 +6836,12 @@
     </row>
     <row r="16" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="47" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="B16" s="47"/>
       <c r="C16" s="47"/>
       <c r="D16" s="47" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E16" s="47"/>
       <c r="F16" s="47" t="s">
@@ -6907,12 +6863,12 @@
     </row>
     <row r="17" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="47" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B17" s="47"/>
       <c r="C17" s="47"/>
       <c r="D17" s="47" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E17" s="47"/>
       <c r="F17" s="47" t="s">
@@ -6934,11 +6890,14 @@
     </row>
     <row r="18" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="47" t="s">
-        <v>283</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="B18" s="47"/>
+      <c r="C18" s="47"/>
       <c r="D18" s="47" t="s">
-        <v>365</v>
-      </c>
+        <v>364</v>
+      </c>
+      <c r="E18" s="47"/>
       <c r="F18" s="47" t="s">
         <v>240</v>
       </c>
@@ -6951,14 +6910,21 @@
       <c r="I18" s="47" t="b">
         <v>0</v>
       </c>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
     </row>
     <row r="19" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="47" t="s">
-        <v>284</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="B19" s="47"/>
+      <c r="C19" s="47"/>
       <c r="D19" s="47" t="s">
-        <v>366</v>
-      </c>
+        <v>365</v>
+      </c>
+      <c r="E19" s="47"/>
       <c r="F19" s="47" t="s">
         <v>240</v>
       </c>
@@ -6971,17 +6937,18 @@
       <c r="I19" s="47" t="b">
         <v>0</v>
       </c>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+      <c r="M19" s="47"/>
     </row>
     <row r="20" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="47" t="s">
-        <v>285</v>
-      </c>
-      <c r="B20" s="47"/>
-      <c r="C20" s="47"/>
+        <v>286</v>
+      </c>
       <c r="D20" s="47" t="s">
-        <v>367</v>
-      </c>
-      <c r="E20" s="47"/>
+        <v>366</v>
+      </c>
       <c r="F20" s="47" t="s">
         <v>240</v>
       </c>
@@ -6994,21 +6961,14 @@
       <c r="I20" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
-      <c r="L20" s="47"/>
-      <c r="M20" s="47"/>
     </row>
     <row r="21" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="47" t="s">
-        <v>263</v>
-      </c>
-      <c r="B21" s="47"/>
-      <c r="C21" s="47"/>
+        <v>287</v>
+      </c>
       <c r="D21" s="47" t="s">
-        <v>368</v>
-      </c>
-      <c r="E21" s="47"/>
+        <v>367</v>
+      </c>
       <c r="F21" s="47" t="s">
         <v>240</v>
       </c>
@@ -7021,21 +6981,14 @@
       <c r="I21" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
-      <c r="L21" s="47"/>
-      <c r="M21" s="47"/>
     </row>
     <row r="22" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="47" t="s">
-        <v>286</v>
-      </c>
-      <c r="B22" s="47"/>
-      <c r="C22" s="47"/>
+        <v>288</v>
+      </c>
       <c r="D22" s="47" t="s">
-        <v>369</v>
-      </c>
-      <c r="E22" s="47"/>
+        <v>368</v>
+      </c>
       <c r="F22" s="47" t="s">
         <v>240</v>
       </c>
@@ -7048,21 +7001,14 @@
       <c r="I22" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="J22" s="47"/>
-      <c r="K22" s="47"/>
-      <c r="L22" s="47"/>
-      <c r="M22" s="47"/>
     </row>
     <row r="23" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="47" t="s">
-        <v>287</v>
-      </c>
-      <c r="B23" s="47"/>
-      <c r="C23" s="47"/>
+        <v>289</v>
+      </c>
       <c r="D23" s="47" t="s">
-        <v>370</v>
-      </c>
-      <c r="E23" s="47"/>
+        <v>369</v>
+      </c>
       <c r="F23" s="47" t="s">
         <v>240</v>
       </c>
@@ -7075,21 +7021,14 @@
       <c r="I23" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="J23" s="47"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="47"/>
-      <c r="M23" s="47"/>
     </row>
     <row r="24" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="47" t="s">
-        <v>288</v>
-      </c>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
+        <v>290</v>
+      </c>
       <c r="D24" s="47" t="s">
-        <v>371</v>
-      </c>
-      <c r="E24" s="47"/>
+        <v>370</v>
+      </c>
       <c r="F24" s="47" t="s">
         <v>240</v>
       </c>
@@ -7102,17 +7041,13 @@
       <c r="I24" s="47" t="b">
         <v>0</v>
       </c>
-      <c r="J24" s="47"/>
-      <c r="K24" s="47"/>
-      <c r="L24" s="47"/>
-      <c r="M24" s="47"/>
     </row>
     <row r="25" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D25" s="47" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F25" s="47" t="s">
         <v>240</v>
@@ -7129,10 +7064,10 @@
     </row>
     <row r="26" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="47" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D26" s="47" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="F26" s="47" t="s">
         <v>240</v>
@@ -7149,10 +7084,10 @@
     </row>
     <row r="27" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="47" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D27" s="47" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F27" s="47" t="s">
         <v>240</v>
@@ -7169,10 +7104,10 @@
     </row>
     <row r="28" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="47" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D28" s="47" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F28" s="47" t="s">
         <v>240</v>
@@ -7189,10 +7124,10 @@
     </row>
     <row r="29" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="47" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D29" s="47" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="F29" s="47" t="s">
         <v>240</v>
@@ -7209,10 +7144,10 @@
     </row>
     <row r="30" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="47" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D30" s="47" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F30" s="47" t="s">
         <v>240</v>
@@ -7229,10 +7164,10 @@
     </row>
     <row r="31" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="47" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D31" s="47" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="F31" s="47" t="s">
         <v>240</v>
@@ -7249,10 +7184,10 @@
     </row>
     <row r="32" spans="1:13" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="47" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D32" s="47" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F32" s="47" t="s">
         <v>240</v>
@@ -7269,10 +7204,10 @@
     </row>
     <row r="33" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="47" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D33" s="47" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="F33" s="47" t="s">
         <v>240</v>
@@ -7289,10 +7224,10 @@
     </row>
     <row r="34" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="47" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D34" s="47" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="F34" s="47" t="s">
         <v>240</v>
@@ -7309,10 +7244,10 @@
     </row>
     <row r="35" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="47" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D35" s="47" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="F35" s="47" t="s">
         <v>240</v>
@@ -7329,10 +7264,10 @@
     </row>
     <row r="36" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="47" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D36" s="47" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F36" s="47" t="s">
         <v>240</v>
@@ -7349,10 +7284,10 @@
     </row>
     <row r="37" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="47" t="s">
-        <v>301</v>
+        <v>265</v>
       </c>
       <c r="D37" s="47" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="F37" s="47" t="s">
         <v>240</v>
@@ -7369,10 +7304,10 @@
     </row>
     <row r="38" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="47" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="D38" s="47" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F38" s="47" t="s">
         <v>240</v>
@@ -7389,10 +7324,10 @@
     </row>
     <row r="39" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="47" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="D39" s="47" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F39" s="47" t="s">
         <v>240</v>
@@ -7409,10 +7344,10 @@
     </row>
     <row r="40" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="47" t="s">
-        <v>304</v>
+        <v>416</v>
       </c>
       <c r="D40" s="47" t="s">
-        <v>387</v>
+        <v>417</v>
       </c>
       <c r="F40" s="47" t="s">
         <v>240</v>
@@ -7432,7 +7367,7 @@
         <v>305</v>
       </c>
       <c r="D41" s="47" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F41" s="47" t="s">
         <v>240</v>
@@ -7449,10 +7384,10 @@
     </row>
     <row r="42" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="47" t="s">
-        <v>265</v>
+        <v>306</v>
       </c>
       <c r="D42" s="47" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F42" s="47" t="s">
         <v>240</v>
@@ -7469,10 +7404,10 @@
     </row>
     <row r="43" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="47" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="D43" s="47" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F43" s="47" t="s">
         <v>240</v>
@@ -7489,10 +7424,10 @@
     </row>
     <row r="44" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="47" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="D44" s="47" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F44" s="47" t="s">
         <v>240</v>
@@ -7509,10 +7444,10 @@
     </row>
     <row r="45" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="47" t="s">
-        <v>422</v>
+        <v>309</v>
       </c>
       <c r="D45" s="47" t="s">
-        <v>423</v>
+        <v>390</v>
       </c>
       <c r="F45" s="47" t="s">
         <v>240</v>
@@ -7529,10 +7464,10 @@
     </row>
     <row r="46" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="47" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D46" s="47" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F46" s="47" t="s">
         <v>240</v>
@@ -7549,10 +7484,10 @@
     </row>
     <row r="47" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="47" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D47" s="47" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="F47" s="47" t="s">
         <v>240</v>
@@ -7569,10 +7504,10 @@
     </row>
     <row r="48" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="47" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D48" s="47" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F48" s="47" t="s">
         <v>240</v>
@@ -7589,10 +7524,10 @@
     </row>
     <row r="49" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="47" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D49" s="47" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F49" s="47" t="s">
         <v>240</v>
@@ -7609,10 +7544,10 @@
     </row>
     <row r="50" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="47" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="D50" s="47" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F50" s="47" t="s">
         <v>240</v>
@@ -7629,10 +7564,10 @@
     </row>
     <row r="51" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="47" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="D51" s="47" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="F51" s="47" t="s">
         <v>240</v>
@@ -7649,10 +7584,10 @@
     </row>
     <row r="52" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="47" t="s">
-        <v>314</v>
+        <v>266</v>
       </c>
       <c r="D52" s="47" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F52" s="47" t="s">
         <v>240</v>
@@ -7669,10 +7604,10 @@
     </row>
     <row r="53" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="47" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D53" s="47" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="F53" s="47" t="s">
         <v>240</v>
@@ -7689,10 +7624,10 @@
     </row>
     <row r="54" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="47" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D54" s="47" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F54" s="47" t="s">
         <v>240</v>
@@ -7709,10 +7644,10 @@
     </row>
     <row r="55" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="47" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D55" s="47" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F55" s="47" t="s">
         <v>240</v>
@@ -7729,10 +7664,10 @@
     </row>
     <row r="56" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="47" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="D56" s="47" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F56" s="47" t="s">
         <v>240</v>
@@ -7749,10 +7684,10 @@
     </row>
     <row r="57" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="47" t="s">
-        <v>266</v>
+        <v>320</v>
       </c>
       <c r="D57" s="47" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F57" s="47" t="s">
         <v>240</v>
@@ -7769,10 +7704,10 @@
     </row>
     <row r="58" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="47" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D58" s="47" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F58" s="47" t="s">
         <v>240</v>
@@ -7789,10 +7724,10 @@
     </row>
     <row r="59" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="47" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D59" s="47" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F59" s="47" t="s">
         <v>240</v>
@@ -7809,10 +7744,10 @@
     </row>
     <row r="60" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="47" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D60" s="47" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F60" s="47" t="s">
         <v>240</v>
@@ -7829,10 +7764,10 @@
     </row>
     <row r="61" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="47" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D61" s="47" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="F61" s="47" t="s">
         <v>240</v>
@@ -7849,10 +7784,10 @@
     </row>
     <row r="62" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="47" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D62" s="47" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F62" s="47" t="s">
         <v>240</v>
@@ -7869,10 +7804,10 @@
     </row>
     <row r="63" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="47" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D63" s="47" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F63" s="47" t="s">
         <v>240</v>
@@ -7889,10 +7824,10 @@
     </row>
     <row r="64" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="47" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D64" s="47" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F64" s="47" t="s">
         <v>240</v>
@@ -7909,10 +7844,10 @@
     </row>
     <row r="65" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="47" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D65" s="47" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F65" s="47" t="s">
         <v>240</v>
@@ -7927,115 +7862,115 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="47" t="s">
-        <v>327</v>
-      </c>
-      <c r="D66" s="47" t="s">
-        <v>412</v>
-      </c>
-      <c r="F66" s="47" t="s">
-        <v>240</v>
-      </c>
-      <c r="G66" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="H66" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="I66" s="47" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="47" t="s">
-        <v>328</v>
-      </c>
-      <c r="D67" s="47" t="s">
-        <v>413</v>
-      </c>
-      <c r="F67" s="47" t="s">
-        <v>240</v>
-      </c>
-      <c r="G67" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="H67" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="I67" s="47" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="47" t="s">
-        <v>329</v>
-      </c>
-      <c r="D68" s="47" t="s">
-        <v>414</v>
-      </c>
-      <c r="F68" s="47" t="s">
-        <v>240</v>
-      </c>
-      <c r="G68" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="H68" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="I68" s="47" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="47" t="s">
-        <v>330</v>
-      </c>
-      <c r="D69" s="47" t="s">
-        <v>415</v>
-      </c>
-      <c r="F69" s="47" t="s">
-        <v>240</v>
-      </c>
-      <c r="G69" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="H69" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="I69" s="47" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="47" t="s">
+    <row r="66" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="48" t="s">
+        <v>241</v>
+      </c>
+      <c r="D66" s="13" t="s">
         <v>331</v>
       </c>
-      <c r="D70" s="47" t="s">
-        <v>416</v>
-      </c>
-      <c r="F70" s="47" t="s">
-        <v>240</v>
-      </c>
-      <c r="G70" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="H70" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="I70" s="47" t="b">
+      <c r="F66" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="G66" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H66" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I66" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="48" t="s">
+        <v>242</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="F67" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="G67" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H67" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I67" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="48" t="s">
+        <v>243</v>
+      </c>
+      <c r="D68" s="13" t="s">
+        <v>333</v>
+      </c>
+      <c r="F68" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="G68" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H68" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I68" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="48" t="s">
+        <v>244</v>
+      </c>
+      <c r="D69" s="13" t="s">
+        <v>334</v>
+      </c>
+      <c r="F69" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="G69" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H69" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I69" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="48" t="s">
+        <v>245</v>
+      </c>
+      <c r="D70" s="13" t="s">
+        <v>335</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="G70" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="H70" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="I70" s="13" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="48" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="F71" s="13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="G71" s="13" t="b">
         <v>0</v>
@@ -8049,13 +7984,13 @@
     </row>
     <row r="72" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="48" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="D72" s="13" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="F72" s="13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="G72" s="13" t="b">
         <v>0</v>
@@ -8069,13 +8004,13 @@
     </row>
     <row r="73" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="48" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="G73" s="13" t="b">
         <v>0</v>
@@ -8089,13 +8024,13 @@
     </row>
     <row r="74" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="48" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="G74" s="13" t="b">
         <v>0</v>
@@ -8109,13 +8044,13 @@
     </row>
     <row r="75" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="48" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="F75" s="13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="G75" s="13" t="b">
         <v>0</v>
@@ -8129,13 +8064,13 @@
     </row>
     <row r="76" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="48" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="D76" s="13" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="F76" s="13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="G76" s="13" t="b">
         <v>0</v>
@@ -8149,13 +8084,13 @@
     </row>
     <row r="77" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="48" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="F77" s="13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="G77" s="13" t="b">
         <v>0</v>
@@ -8168,14 +8103,14 @@
       </c>
     </row>
     <row r="78" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="48" t="s">
-        <v>248</v>
+      <c r="A78" s="13" t="s">
+        <v>253</v>
       </c>
       <c r="D78" s="13" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="G78" s="13" t="b">
         <v>0</v>
@@ -8188,14 +8123,14 @@
       </c>
     </row>
     <row r="79" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="48" t="s">
-        <v>249</v>
+      <c r="A79" s="13" t="s">
+        <v>254</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="G79" s="13" t="b">
         <v>0</v>
@@ -8208,14 +8143,14 @@
       </c>
     </row>
     <row r="80" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="48" t="s">
-        <v>250</v>
+      <c r="A80" s="13" t="s">
+        <v>255</v>
       </c>
       <c r="D80" s="13" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="G80" s="13" t="b">
         <v>0</v>
@@ -8228,14 +8163,14 @@
       </c>
     </row>
     <row r="81" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="48" t="s">
-        <v>251</v>
+      <c r="A81" s="13" t="s">
+        <v>256</v>
       </c>
       <c r="D81" s="13" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="F81" s="13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="G81" s="13" t="b">
         <v>0</v>
@@ -8248,14 +8183,14 @@
       </c>
     </row>
     <row r="82" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="48" t="s">
-        <v>252</v>
+      <c r="A82" s="13" t="s">
+        <v>257</v>
       </c>
       <c r="D82" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="F82" s="13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="G82" s="13" t="b">
         <v>0</v>
@@ -8269,13 +8204,13 @@
     </row>
     <row r="83" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>253</v>
+        <v>258</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="F83" s="13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="G83" s="13" t="b">
         <v>0</v>
@@ -8289,13 +8224,13 @@
     </row>
     <row r="84" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
-        <v>254</v>
+        <v>419</v>
       </c>
       <c r="D84" s="13" t="s">
-        <v>347</v>
+        <v>420</v>
       </c>
       <c r="F84" s="13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="G84" s="13" t="b">
         <v>0</v>
@@ -8306,16 +8241,20 @@
       <c r="I84" s="13" t="b">
         <v>0</v>
       </c>
+      <c r="J84" s="48"/>
+      <c r="K84" s="48"/>
+      <c r="L84" s="48"/>
+      <c r="M84" s="48"/>
     </row>
     <row r="85" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>255</v>
+        <v>421</v>
       </c>
       <c r="D85" s="13" t="s">
-        <v>348</v>
+        <v>422</v>
       </c>
       <c r="F85" s="13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="G85" s="13" t="b">
         <v>0</v>
@@ -8326,16 +8265,20 @@
       <c r="I85" s="13" t="b">
         <v>0</v>
       </c>
+      <c r="J85" s="48"/>
+      <c r="K85" s="48"/>
+      <c r="L85" s="48"/>
+      <c r="M85" s="48"/>
     </row>
     <row r="86" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="13" t="s">
-        <v>256</v>
+      <c r="A86" s="48" t="s">
+        <v>425</v>
       </c>
       <c r="D86" s="13" t="s">
-        <v>349</v>
+        <v>427</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="G86" s="13" t="b">
         <v>0</v>
@@ -8348,14 +8291,14 @@
       </c>
     </row>
     <row r="87" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="13" t="s">
-        <v>257</v>
+      <c r="A87" s="48" t="s">
+        <v>426</v>
       </c>
       <c r="D87" s="13" t="s">
-        <v>350</v>
+        <v>428</v>
       </c>
       <c r="F87" s="13" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="G87" s="13" t="b">
         <v>0</v>
@@ -8367,113 +8310,50 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="D88" s="13" t="s">
-        <v>351</v>
-      </c>
-      <c r="F88" s="13" t="s">
-        <v>417</v>
-      </c>
-      <c r="G88" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H88" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I88" s="13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="13" t="s">
-        <v>425</v>
-      </c>
-      <c r="D89" s="13" t="s">
-        <v>426</v>
-      </c>
-      <c r="F89" s="13" t="s">
-        <v>417</v>
-      </c>
-      <c r="G89" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H89" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I89" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="J89" s="48"/>
-      <c r="K89" s="48"/>
-      <c r="L89" s="48"/>
-      <c r="M89" s="48"/>
-    </row>
-    <row r="90" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="13" t="s">
-        <v>427</v>
-      </c>
-      <c r="D90" s="13" t="s">
-        <v>428</v>
-      </c>
-      <c r="F90" s="13" t="s">
-        <v>417</v>
-      </c>
-      <c r="G90" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H90" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I90" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="J90" s="48"/>
-      <c r="K90" s="48"/>
-      <c r="L90" s="48"/>
-      <c r="M90" s="48"/>
-    </row>
-    <row r="91" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="48" t="s">
-        <v>431</v>
-      </c>
-      <c r="D91" s="13" t="s">
-        <v>433</v>
-      </c>
-      <c r="F91" s="13" t="s">
-        <v>417</v>
-      </c>
-      <c r="G91" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H91" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I91" s="13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="48" t="s">
-        <v>432</v>
-      </c>
-      <c r="D92" s="13" t="s">
-        <v>434</v>
-      </c>
-      <c r="F92" s="13" t="s">
-        <v>417</v>
-      </c>
-      <c r="G92" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="H92" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="I92" s="13" t="b">
-        <v>0</v>
-      </c>
+    <row r="88" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="14"/>
+      <c r="B88" s="20"/>
+      <c r="D88" s="14"/>
+      <c r="F88" s="14"/>
+      <c r="G88" s="14"/>
+      <c r="H88" s="14"/>
+      <c r="I88" s="14"/>
+    </row>
+    <row r="89" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="14"/>
+      <c r="B89" s="20"/>
+      <c r="D89" s="14"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="14"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="14"/>
+    </row>
+    <row r="90" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="14"/>
+      <c r="B90" s="20"/>
+      <c r="D90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
+    </row>
+    <row r="91" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="14"/>
+      <c r="B91" s="20"/>
+      <c r="D91" s="14"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="14"/>
+    </row>
+    <row r="92" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="14"/>
+      <c r="B92" s="20"/>
+      <c r="D92" s="14"/>
+      <c r="F92" s="14"/>
+      <c r="G92" s="14"/>
+      <c r="H92" s="14"/>
+      <c r="I92" s="14"/>
     </row>
     <row r="93" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="14"/>
@@ -8691,46 +8571,56 @@
       <c r="H116" s="14"/>
       <c r="I116" s="14"/>
     </row>
-    <row r="117" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="14"/>
       <c r="B117" s="20"/>
+      <c r="C117" s="21"/>
       <c r="D117" s="14"/>
+      <c r="E117" s="21"/>
       <c r="F117" s="14"/>
       <c r="G117" s="14"/>
       <c r="H117" s="14"/>
       <c r="I117" s="14"/>
     </row>
-    <row r="118" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="14"/>
       <c r="B118" s="20"/>
+      <c r="C118" s="21"/>
       <c r="D118" s="14"/>
+      <c r="E118" s="21"/>
       <c r="F118" s="14"/>
       <c r="G118" s="14"/>
       <c r="H118" s="14"/>
       <c r="I118" s="14"/>
     </row>
-    <row r="119" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="14"/>
       <c r="B119" s="20"/>
+      <c r="C119" s="21"/>
       <c r="D119" s="14"/>
+      <c r="E119" s="21"/>
       <c r="F119" s="14"/>
       <c r="G119" s="14"/>
       <c r="H119" s="14"/>
       <c r="I119" s="14"/>
     </row>
-    <row r="120" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="14"/>
       <c r="B120" s="20"/>
+      <c r="C120" s="21"/>
       <c r="D120" s="14"/>
+      <c r="E120" s="21"/>
       <c r="F120" s="14"/>
       <c r="G120" s="14"/>
       <c r="H120" s="14"/>
       <c r="I120" s="14"/>
     </row>
-    <row r="121" spans="1:9" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="14"/>
       <c r="B121" s="20"/>
+      <c r="C121" s="21"/>
       <c r="D121" s="14"/>
+      <c r="E121" s="21"/>
       <c r="F121" s="14"/>
       <c r="G121" s="14"/>
       <c r="H121" s="14"/>
@@ -8746,61 +8636,6 @@
       <c r="G122" s="14"/>
       <c r="H122" s="14"/>
       <c r="I122" s="14"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A123" s="14"/>
-      <c r="B123" s="20"/>
-      <c r="C123" s="21"/>
-      <c r="D123" s="14"/>
-      <c r="E123" s="21"/>
-      <c r="F123" s="14"/>
-      <c r="G123" s="14"/>
-      <c r="H123" s="14"/>
-      <c r="I123" s="14"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="14"/>
-      <c r="B124" s="20"/>
-      <c r="C124" s="21"/>
-      <c r="D124" s="14"/>
-      <c r="E124" s="21"/>
-      <c r="F124" s="14"/>
-      <c r="G124" s="14"/>
-      <c r="H124" s="14"/>
-      <c r="I124" s="14"/>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="14"/>
-      <c r="B125" s="20"/>
-      <c r="C125" s="21"/>
-      <c r="D125" s="14"/>
-      <c r="E125" s="21"/>
-      <c r="F125" s="14"/>
-      <c r="G125" s="14"/>
-      <c r="H125" s="14"/>
-      <c r="I125" s="14"/>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A126" s="14"/>
-      <c r="B126" s="20"/>
-      <c r="C126" s="21"/>
-      <c r="D126" s="14"/>
-      <c r="E126" s="21"/>
-      <c r="F126" s="14"/>
-      <c r="G126" s="14"/>
-      <c r="H126" s="14"/>
-      <c r="I126" s="14"/>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A127" s="14"/>
-      <c r="B127" s="20"/>
-      <c r="C127" s="21"/>
-      <c r="D127" s="14"/>
-      <c r="E127" s="21"/>
-      <c r="F127" s="14"/>
-      <c r="G127" s="14"/>
-      <c r="H127" s="14"/>
-      <c r="I127" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added ability to perform costing of upgrades, addresses #41. Latest measures.
</commit_message>
<xml_diff>
--- a/projects/resstock_testing.xlsx
+++ b/projects/resstock_testing.xlsx
@@ -6046,13 +6046,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C8" s="39" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="E8" s="39" t="s">
         <v>234</v>
@@ -6082,13 +6082,13 @@
         <v>1</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C9" s="39" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="E9" s="39" t="s">
         <v>234</v>

</xml_diff>